<commit_message>
Fixed two FCS filenames for compensation controls from NHLBI.
</commit_message>
<xml_diff>
--- a/NHLBI.xlsx
+++ b/NHLBI.xlsx
@@ -265,12 +265,6 @@
     <t>Compensation Controls_V545 Stained Control.fcs</t>
   </si>
   <si>
-    <t>6:Compensation Controls_CD11c PE-Cy7 G780 Stained Control.fcs</t>
-  </si>
-  <si>
-    <t>4:Compensation Controls_CCR6 PE-Cy7 G780 Stained Control.fcs</t>
-  </si>
-  <si>
     <t>LIVE GREEN:B515</t>
   </si>
   <si>
@@ -317,6 +311,12 @@
   </si>
   <si>
     <t>HLA-DR:V545</t>
+  </si>
+  <si>
+    <t>Compensation Controls_CD11c PE-Cy7 G780 Stained Control.fcs</t>
+  </si>
+  <si>
+    <t>Compensation Controls_CCR6 PE-Cy7 G780 Stained Control.fcs</t>
   </si>
 </sst>
 </file>
@@ -931,7 +931,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -991,7 +991,7 @@
         <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -1014,7 +1014,7 @@
         <v>77</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -1037,7 +1037,7 @@
         <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -1060,7 +1060,7 @@
         <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -1083,7 +1083,7 @@
         <v>69</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
@@ -1106,7 +1106,7 @@
         <v>72</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C9" t="s">
         <v>10</v>
@@ -1126,10 +1126,10 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="B10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C10" t="s">
         <v>11</v>
@@ -1149,10 +1149,10 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -1175,7 +1175,7 @@
         <v>73</v>
       </c>
       <c r="B12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C12" t="s">
         <v>13</v>
@@ -1198,7 +1198,7 @@
         <v>76</v>
       </c>
       <c r="B13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
@@ -1221,7 +1221,7 @@
         <v>70</v>
       </c>
       <c r="B14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
@@ -1244,7 +1244,7 @@
         <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C15" t="s">
         <v>8</v>
@@ -1267,7 +1267,7 @@
         <v>71</v>
       </c>
       <c r="B16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C16" t="s">
         <v>10</v>
@@ -1290,7 +1290,7 @@
         <v>78</v>
       </c>
       <c r="B17" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C17" t="s">
         <v>11</v>
@@ -1313,7 +1313,7 @@
         <v>79</v>
       </c>
       <c r="B18" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C18" t="s">
         <v>2</v>
@@ -1336,7 +1336,7 @@
         <v>80</v>
       </c>
       <c r="B19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C19" t="s">
         <v>2</v>

</xml_diff>